<commit_message>
Se extrajo la informacion de la bibliografia restante. Se sumaron las materias de tuped que faltaban, queda separar tituolos y autores
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas.xlsx
+++ b/data/procesados/bibliografia_programas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCF0EDB-CABE-426D-A136-EA365770434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D69D36-B0ED-407A-BF8A-616644AF3BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="97">
   <si>
     <t>Carrera</t>
   </si>
@@ -275,6 +275,72 @@
   </si>
   <si>
     <t>GROSSMAN, Stanley (2008): “Algebra Lineal”.- MacGraw Hill, México Sexta edición.</t>
+  </si>
+  <si>
+    <t>Algoritmos y Estructuras de Datos - TUPED</t>
+  </si>
+  <si>
+    <t>Aho, A. V., Hopcroft, J. E., &amp; Ullman, J. D. (1998). Estructuras de datos y algoritmos (A. Vargas Villazón &amp; J. Lozano Moreno, Trads.; 1.a ed.). Pearson Educación.</t>
+  </si>
+  <si>
+    <t>Bhargava, A. (2016). Grokking Algorithms: An Illustrated Guide for Programmers and Other Curious People.</t>
+  </si>
+  <si>
+    <t>Cormen, T. H., Leiserson, C. E., Rivest, R. L., &amp; Stein, C. (2022). Introduction to algorithms (Fourth edition). The MIT Press.</t>
+  </si>
+  <si>
+    <t>Kok, A. S. (2019). Hands-On Blockchain for Python Developers: Gain blockchain programming skills to build decentralized applications using Python. Packt Publishing Ltd.</t>
+  </si>
+  <si>
+    <t>Miller, B., &amp; Ranum, D. (2013). Solución de problemas con algoritmos y estructuras de datos usando Python (M. Orozco-Alzate, Trad.; 2.a ed.).</t>
+  </si>
+  <si>
+    <t>Aspectos Legales del Uso de la Información - TUPED</t>
+  </si>
+  <si>
+    <t>“Tratado de Derecho Constitucional”, ROSATTI Horacio, 2° edición ampliada, Rubinzal Culzoni Editores, Santa Fé 2017.</t>
+  </si>
+  <si>
+    <t>“Código Civil y Comercial de la Nación comentado”, dirigido por Ricardo Luis LORENZETTI, 1° edición, Rubinzal Culzoni Editores, Santa Fé, 2014.</t>
+  </si>
+  <si>
+    <t>“Derecho Procesal Administrativo”, HUTCHINSON Tomás, 1° edición, Rubinzal Culzoni Editores, Santa Fé 2009.</t>
+  </si>
+  <si>
+    <t>“Acerca de la reflexión humana. La necesidad de detenernos y partir de la ignorancia”, Guillermo MAGI, Fundación La Hendija, 1° edición, 2016.</t>
+  </si>
+  <si>
+    <t>“Tratado de derecho administrativo y obras selectas”, GORDILLO Agustín, Tomo 1, Parte general, 11a ed., Buenos Aires, F.D.A., 2013.</t>
+  </si>
+  <si>
+    <t>Desregulación, Entre el Derecho y la Economía, Jorge Eduardo BUSTAMANTE, Editorial Abeledo Perrot, Buenos Aires, 1993.</t>
+  </si>
+  <si>
+    <t>Sistema económico y rentístico, ALBERDI, Juan B., Editorial Ciudad Argentina, Buenos Aires, 1998.</t>
+  </si>
+  <si>
+    <t>“Manual De Derecho Procesal Civil”, Lino E. Palacio Actualizador: Carlos E. Camps , Luis E. Palacio , Lino A. Palacio , Editorial Abeledo Perrot, Edicion 2016.</t>
+  </si>
+  <si>
+    <t>“Contratos administrativos”, SILVA CENSIO, Jorge A., Astrea, Buenos Aires, 1982.</t>
+  </si>
+  <si>
+    <t>Nuevos Principios de Comercio Internacional, Para actuar en Escenarios Globalizados, LEDESMA Carlos A., Ediciones Macchi, 5° edición, 1997.</t>
+  </si>
+  <si>
+    <t>Probabilidad y Estadística - TUPED</t>
+  </si>
+  <si>
+    <t>* MENDENHALL, W.: Introducción a la probabilidad y estadística., México DF: Cengage Learning Editores, SA de CV (2010).</t>
+  </si>
+  <si>
+    <t>* RAMOS, EVA: Estadística para todos. Ediciones Pirámide (2016)</t>
+  </si>
+  <si>
+    <t>* GUTIERREZ BANEGAS, A. L. y SABARIA, L.: Probabilidad y estadística: enfoque por competencias. McGraw - Hill (2012)</t>
+  </si>
+  <si>
+    <t>McGraw - Hill (2012)</t>
   </si>
 </sst>
 </file>
@@ -646,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1638,215 @@
         <v>73</v>
       </c>
     </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>75</v>
+      </c>
+      <c r="C88" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
+        <v>81</v>
+      </c>
+      <c r="C93" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>81</v>
+      </c>
+      <c r="C98" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>92</v>
+      </c>
+      <c r="C100" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
NOTAS y modificacion de xlsx
</commit_message>
<xml_diff>
--- a/data/procesados/bibliografia_programas.xlsx
+++ b/data/procesados/bibliografia_programas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D69D36-B0ED-407A-BF8A-616644AF3BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C5B74-D535-4ED7-BB83-D94BE27647ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="93">
   <si>
     <t>Carrera</t>
   </si>
@@ -40,57 +40,12 @@
     <t>Licenciatura en Bioinformática</t>
   </si>
   <si>
-    <t>Comprensión Lectora y Producción Escrita - Bioinformática</t>
-  </si>
-  <si>
-    <t>Los materiales que se mencionan a continuación, se encontrarán disponibles para los alumnos -siempre que
-sea posible- en el sitio de la cátedra, dentro del Campus virtual de la FIUNER.
-Se utilizará como material obligatorio el Cuadernillo de la asignatura, que ha sido elaborado por la cátedra.
-En él se abordan los contenidos de la materia y se presentan las actividades prácticas a desarrollar durante
-el cursado.</t>
-  </si>
-  <si>
     <t>Bioingeniería</t>
   </si>
   <si>
-    <t>Comprensión Lectora y Producción Escrita - Bioingeniería</t>
-  </si>
-  <si>
     <t>Ingeniería en Transporte</t>
   </si>
   <si>
-    <t>Comprensión Lectora y Producción Escrita - Transporte</t>
-  </si>
-  <si>
-    <t>Comprensión Lectora y Producción Escrita - TUPED</t>
-  </si>
-  <si>
-    <t>Los materiales se encontrarán disponibles para los alumnos -siempre que sea posible- en el sitio de la
-cátedra, dentro del Campus virtual de la FIUNER.
-Se utilizará como material obligatorio el Cuadernillo de la asignatura, que ha sido elaborado por la cátedra.
-En él se abordan los contenidos de la materia y se presentan las actividades prácticas a desarrollar durante
-el cursado.
-Bibliografía utilizada para la realización de esta planificación:
-ÁLVAREZ MÉNDEZ, J. M. (2003): La evaluación a examen. Bs. As.: Miño y Dávila.
-CARLINO, P. (2005). Escribir, leer y aprender en la Universidad. Una introducción a la alfabetización
-académica. Buenos Aires, Fondo de Cultura Económica.
-CARLINO, P. (2013) Alfabetización académica 10 años después. Revista Mexicana de Investigación
-Educativa Vol. 18, Núm. 57, Pp. 355-381 Disponible en: http://www.redalyc.org/pdf/140/14025774003.pdf
-CASTELLÓ, M. (2014). Los retos actuales de la alfabetización académica: estado de la cuestión y últimas
-investigaciones. Revista Enunciación, Vol 19, Núm. 2, Pp. 346-365. Disponible en:
-http://revistas.udistrital.edu.co/ojs/index.php/enunc/article/view/8256
-CORCELLES SEUBA, M. y OLIVA GIRBAU, A. (2016) “La escritura colaborativa de textos académicos: un
-proyecto en el aula de Psicología de la educación” En BAÑALES, G., CASTELLÓ M., y VEGA N. A. (Eds.).
-Enseñar a leer y escribir en la educación superior. Propuestas educativas basadas en la investigación.
-México: Ediciones SM. Disponible en:
-http://www.fundacion-sm.org.mx/sites/default/files/Ense%C3%B1ar%20a%20leer%20y%20escribir.pdf
-NARVAJA DE ARNOUX, E.; DI STEFANO, M.; PEREIRA, C (2002). La lectura y la escritura en la
-universidad. Buenos Aires, EUDEBA
-WILLIAM, D. (2009): Una síntesis integradora de la investigación e implicancias para una nueva teoría de la
-evaluación formativa. En Revista Archivos de Ciencias de la Educación, Año 3, Nº 3, Bs. As., pp: 15-44.
-Disponible en http://www.memoria.fahce.unlp.edu.ar/art_revistas/pr.4080/pr.4080.pdf</t>
-  </si>
-  <si>
     <t>Cálculo en una Variable - Bioinformática</t>
   </si>
   <si>
@@ -154,23 +109,6 @@
     <t>Álgebra Lineal y Geometría Analítica - Transporte</t>
   </si>
   <si>
-    <t>PRECÁLCULO - James Stewart - Sexta Edición</t>
-  </si>
-  <si>
-    <t>Cálculo en una Variable - James Stewart - Séptima Edición</t>
-  </si>
-  <si>
-    <t>Álgebra lineal - Grossman - Séptima edición</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• STEWART, James, (2012): “Cálculo de una variable- Trascendentes y tempranas” - 7ma edición -
-Cengage – Learning – México.
-</t>
-  </si>
-  <si>
-    <t>• STEWART, James, (2012): “Precálculo - Matemáticas para el cálculo” – Sexta edición</t>
-  </si>
-  <si>
     <t>La Biblioteca Estándar de Python. Python Software Foundation</t>
   </si>
   <si>
@@ -180,10 +118,6 @@
     <t>El tutorial de Python. Python Software Foundation.</t>
   </si>
   <si>
-    <t>• STEWART, James, (2012): “Cálculo de una variable- Trascendentes y tempranas” - 7ma edición -
-Cengage – Learning – México</t>
-  </si>
-  <si>
     <t>Sears-Zemansky Física universitaria volumen 1. YOUNG, HUGH D.</t>
   </si>
   <si>
@@ -341,6 +275,30 @@
   </si>
   <si>
     <t>McGraw - Hill (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Álgebra lineal $ Grossman </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRECÁLCULO $ James Stewart </t>
+  </si>
+  <si>
+    <t>Cálculo en una Variable $ James Stewart</t>
+  </si>
+  <si>
+    <t>STEWART, James $ Cálculo de una variable- Trascendentes y tempranas</t>
+  </si>
+  <si>
+    <t>STEWART, James $ Precálculo - Matemáticas para el cálculo</t>
+  </si>
+  <si>
+    <t>El tutorial de Python. $ Python Software Foundation.</t>
+  </si>
+  <si>
+    <t>La Biblioteca Estándar de Python. $ Python Software Foundation</t>
+  </si>
+  <si>
+    <t>Referencia del Lenguaje Python. $ Python Software Foundation.</t>
   </si>
 </sst>
 </file>
@@ -712,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +702,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,348 +724,348 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="C7" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" t="s">
-        <v>47</v>
+        <v>18</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>49</v>
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,43 +1073,43 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1117,10 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,186 +1128,186 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" t="s">
-        <v>52</v>
+        <v>21</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>59</v>
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" t="s">
-        <v>53</v>
+        <v>24</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" t="s">
-        <v>60</v>
+        <v>24</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,10 +1315,10 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,10 +1326,10 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1379,10 +1337,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1390,10 +1348,10 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1401,10 +1359,10 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,230 +1370,230 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="C81" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="C82" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="C83" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1643,10 +1601,10 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>75</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
+      </c>
+      <c r="C84" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1654,10 +1612,10 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1665,10 +1623,10 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C86" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1676,10 +1634,10 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1687,10 +1645,10 @@
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1698,10 +1656,10 @@
         <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1709,10 +1667,10 @@
         <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,10 +1678,10 @@
         <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C91" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1731,10 +1689,10 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1742,10 +1700,10 @@
         <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C93" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1753,10 +1711,10 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1764,10 +1722,10 @@
         <v>3</v>
       </c>
       <c r="B95" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
         <v>81</v>
-      </c>
-      <c r="C95" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1775,10 +1733,10 @@
         <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C96" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1786,10 +1744,10 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C97" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1797,54 +1755,10 @@
         <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C98" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" t="s">
-        <v>92</v>
-      </c>
-      <c r="C99" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" t="s">
-        <v>92</v>
-      </c>
-      <c r="C100" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" t="s">
-        <v>92</v>
-      </c>
-      <c r="C101" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" t="s">
-        <v>92</v>
-      </c>
-      <c r="C102" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>